<commit_message>
international analysis section done
</commit_message>
<xml_diff>
--- a/Thesis/write up/data/Index Description.xlsx
+++ b/Thesis/write up/data/Index Description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielrambanapasi/Desktop/Much Ado Dividends/Much-Ado-Dividends/Thesis/write up/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C316F7D-21D5-834A-A0BD-517C5C4DA552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEFCDAF-4881-DC4B-9764-1A53E00038DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{FE5574C1-C9B5-1642-8B16-412891BE9ED0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>FUDP</t>
   </si>
@@ -149,78 +149,6 @@
     <t>FTSE/JSE Dividend+ Index Total Return Index</t>
   </si>
   <si>
-    <t xml:space="preserve">TICKER </t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK </t>
-  </si>
-  <si>
-    <t>EM</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>EU</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>Codename</t>
-  </si>
-  <si>
-    <t>UK_HY</t>
-  </si>
-  <si>
-    <t>EM_HY</t>
-  </si>
-  <si>
-    <t>JP_HY</t>
-  </si>
-  <si>
-    <t>US_HY</t>
-  </si>
-  <si>
-    <t>W_HY</t>
-  </si>
-  <si>
-    <t>EU_DG</t>
-  </si>
-  <si>
-    <t>JP_DG</t>
-  </si>
-  <si>
-    <t>US_DG</t>
-  </si>
-  <si>
-    <t>SA_DG</t>
-  </si>
-  <si>
-    <t>SA_HY</t>
-  </si>
-  <si>
-    <t>EU_HY</t>
-  </si>
-  <si>
-    <t>UK_B</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>EU_2</t>
-  </si>
-  <si>
-    <t>US_2</t>
-  </si>
-  <si>
     <t>MSCI UK HY Gross Total Return USD Index</t>
   </si>
   <si>
@@ -242,7 +170,10 @@
     <t>S&amp;P EU 350 Dividends Aristocrats Total Return Index</t>
   </si>
   <si>
-    <t>Inception Dates</t>
+    <t xml:space="preserve">Ticker </t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -298,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -444,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,295 +525,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6C965C-7E0C-404B-9A81-C29D4ACD0BAB}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="68.6640625" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>